<commit_message>
v 1.0.5 (fixed structure of file, fixed width of columns in output file)
</commit_message>
<xml_diff>
--- a/outputTimesheet.xlsx
+++ b/outputTimesheet.xlsx
@@ -407,7 +407,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" customWidth="1" width="15"/>
+    <col min="3" max="3" customWidth="1" width="10"/>
+    <col min="4" max="4" customWidth="1" width="25"/>
+    <col min="5" max="5" customWidth="1" width="20"/>
+    <col min="6" max="6" customWidth="1" width="20"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>